<commit_message>
Added subgenre column to data table and modified the code
</commit_message>
<xml_diff>
--- a/movie_review_system/rated_movies.xlsx
+++ b/movie_review_system/rated_movies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macuz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\nai-1-python-grinder\movie_review_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B07D544-4F4D-46DB-9884-18C7008688FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1875220-E7E4-4BEC-8B41-B0A5E6788DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="196">
   <si>
     <t>Reviewer</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Breaking Bad</t>
   </si>
   <si>
-    <t>Forest Gump</t>
-  </si>
-  <si>
     <t>Diuna 2</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>Wilk z Wall Street</t>
   </si>
   <si>
-    <t>Marsjanin</t>
-  </si>
-  <si>
     <t>MoonFall</t>
   </si>
   <si>
@@ -412,9 +406,6 @@
     <t>mordercza opona</t>
   </si>
   <si>
-    <t>pixele</t>
-  </si>
-  <si>
     <t>Arrival</t>
   </si>
   <si>
@@ -607,10 +598,16 @@
     <t>fantasy</t>
   </si>
   <si>
-    <t>Maksymilian Mrówka</t>
-  </si>
-  <si>
-    <t>The Sopranos</t>
+    <t>Subgenre</t>
+  </si>
+  <si>
+    <t>sitcom</t>
+  </si>
+  <si>
+    <t>historyczny</t>
+  </si>
+  <si>
+    <t>thriller</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1013,7 @@
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1024,13 +1021,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1041,10 +1041,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1055,10 +1058,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1069,10 +1072,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1083,10 +1089,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1097,10 +1106,13 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1111,10 +1123,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1125,10 +1140,13 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1139,10 +1157,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1153,10 +1174,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1167,10 +1191,13 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1181,10 +1208,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1195,10 +1225,13 @@
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1209,10 +1242,13 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1223,10 +1259,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1237,10 +1276,10 @@
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1251,10 +1290,13 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1265,10 +1307,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1279,10 +1324,13 @@
         <v>9</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1293,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1307,10 +1355,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1321,10 +1369,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,10 +1383,13 @@
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1349,10 +1400,13 @@
         <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E24" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1363,10 +1417,10 @@
         <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1377,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1391,10 +1445,13 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1405,10 +1462,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1419,10 +1479,13 @@
         <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1433,10 +1496,13 @@
         <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1447,10 +1513,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1461,10 +1527,13 @@
         <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -1475,10 +1544,13 @@
         <v>10</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -1489,10 +1561,13 @@
         <v>8</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1505,8 +1580,11 @@
       <c r="D35" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -1517,10 +1595,10 @@
         <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -1531,10 +1609,13 @@
         <v>9</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
@@ -1545,10 +1626,13 @@
         <v>8</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="E38" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -1559,10 +1643,13 @@
         <v>9</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
@@ -1573,10 +1660,13 @@
         <v>9</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="E40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -1587,10 +1677,13 @@
         <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1601,10 +1694,13 @@
         <v>10</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E42" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1615,10 +1711,13 @@
         <v>9</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E43" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -1629,10 +1728,13 @@
         <v>10</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E44" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1643,10 +1745,13 @@
         <v>10</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1657,10 +1762,13 @@
         <v>10</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1671,10 +1779,13 @@
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1685,10 +1796,13 @@
         <v>10</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1699,10 +1813,13 @@
         <v>10</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1713,10 +1830,13 @@
         <v>9</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1727,10 +1847,13 @@
         <v>8</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="E51" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1741,10 +1864,13 @@
         <v>10</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
@@ -1755,10 +1881,13 @@
         <v>7</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1769,10 +1898,13 @@
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1783,10 +1915,13 @@
         <v>7</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
@@ -1797,10 +1932,13 @@
         <v>9</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
@@ -1811,10 +1949,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
@@ -1825,10 +1963,10 @@
         <v>7</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>3</v>
       </c>
@@ -1839,10 +1977,13 @@
         <v>8</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1853,10 +1994,10 @@
         <v>9</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>3</v>
       </c>
@@ -1867,10 +2008,13 @@
         <v>10</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E61" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
@@ -1881,10 +2025,13 @@
         <v>8</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
@@ -1895,10 +2042,13 @@
         <v>9</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1909,10 +2059,13 @@
         <v>8</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>3</v>
       </c>
@@ -1923,10 +2076,13 @@
         <v>7</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E65" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -1937,10 +2093,13 @@
         <v>10</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
@@ -1951,10 +2110,13 @@
         <v>8</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E67" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -1965,10 +2127,13 @@
         <v>10</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
@@ -1979,10 +2144,13 @@
         <v>9</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E69" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,10 +2161,13 @@
         <v>10</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E70" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -2007,10 +2178,13 @@
         <v>8</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E71" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -2021,10 +2195,10 @@
         <v>10</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -2035,10 +2209,13 @@
         <v>7</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E73" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -2049,10 +2226,13 @@
         <v>2</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>4</v>
       </c>
@@ -2063,10 +2243,10 @@
         <v>6</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
@@ -2077,10 +2257,13 @@
         <v>9</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E76" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -2091,10 +2274,13 @@
         <v>10</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -2105,10 +2291,13 @@
         <v>8</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E78" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
@@ -2119,10 +2308,13 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E79" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>4</v>
       </c>
@@ -2133,10 +2325,13 @@
         <v>8</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E80" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -2147,10 +2342,13 @@
         <v>4</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E81" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>4</v>
       </c>
@@ -2161,10 +2359,10 @@
         <v>7</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
@@ -2175,10 +2373,13 @@
         <v>7</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
@@ -2189,10 +2390,13 @@
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E84" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -2203,10 +2407,13 @@
         <v>8</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E85" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -2214,13 +2421,16 @@
         <v>96</v>
       </c>
       <c r="C86" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
@@ -2228,32 +2438,38 @@
         <v>97</v>
       </c>
       <c r="C87" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E87" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>98</v>
+      <c r="B88" s="3">
+        <v>1670</v>
       </c>
       <c r="C88" s="3">
         <v>10</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E88" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="3">
-        <v>1670</v>
+      <c r="B89" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C89" s="3">
         <v>10</v>
@@ -2262,7 +2478,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -2270,13 +2486,16 @@
         <v>99</v>
       </c>
       <c r="C90" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E90" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
@@ -2284,27 +2503,33 @@
         <v>100</v>
       </c>
       <c r="C91" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C92" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E92" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
@@ -2312,13 +2537,16 @@
         <v>102</v>
       </c>
       <c r="C93" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E93" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>6</v>
       </c>
@@ -2326,13 +2554,16 @@
         <v>103</v>
       </c>
       <c r="C94" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E94" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>6</v>
       </c>
@@ -2340,13 +2571,16 @@
         <v>104</v>
       </c>
       <c r="C95" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E95" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>6</v>
       </c>
@@ -2354,13 +2588,16 @@
         <v>105</v>
       </c>
       <c r="C96" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E96" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>6</v>
       </c>
@@ -2368,13 +2605,16 @@
         <v>106</v>
       </c>
       <c r="C97" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E97" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>6</v>
       </c>
@@ -2382,13 +2622,16 @@
         <v>107</v>
       </c>
       <c r="C98" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E98" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>6</v>
       </c>
@@ -2399,38 +2642,44 @@
         <v>8</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C100" s="3">
-        <v>8</v>
+      <c r="C100" s="4">
+        <v>7</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E100" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C101" s="4">
+      <c r="C101" s="3">
         <v>7</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E101" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>6</v>
       </c>
@@ -2438,13 +2687,16 @@
         <v>111</v>
       </c>
       <c r="C102" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E102" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -2452,13 +2704,16 @@
         <v>112</v>
       </c>
       <c r="C103" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E103" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
@@ -2466,13 +2721,16 @@
         <v>113</v>
       </c>
       <c r="C104" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E104" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -2480,15 +2738,18 @@
         <v>114</v>
       </c>
       <c r="C105" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E105" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>115</v>
@@ -2499,8 +2760,11 @@
       <c r="D106" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E106" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>7</v>
       </c>
@@ -2508,13 +2772,16 @@
         <v>116</v>
       </c>
       <c r="C107" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E107" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -2522,13 +2789,16 @@
         <v>117</v>
       </c>
       <c r="C108" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E108" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
@@ -2536,41 +2806,50 @@
         <v>118</v>
       </c>
       <c r="C109" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E109" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E110" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C110" s="3">
-        <v>7</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="C111" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E111" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -2578,13 +2857,16 @@
         <v>120</v>
       </c>
       <c r="C112" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E112" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>7</v>
       </c>
@@ -2592,13 +2874,16 @@
         <v>121</v>
       </c>
       <c r="C113" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="E113" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>7</v>
       </c>
@@ -2606,55 +2891,67 @@
         <v>122</v>
       </c>
       <c r="C114" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E114" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>123</v>
+      <c r="B115" s="3">
+        <v>2012</v>
       </c>
       <c r="C115" s="3">
         <v>6</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E115" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C116" s="3">
+        <v>3</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E116" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C116" s="3">
-        <v>8</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B117" s="3">
-        <v>2012</v>
-      </c>
       <c r="C117" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E117" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>7</v>
       </c>
@@ -2662,13 +2959,13 @@
         <v>125</v>
       </c>
       <c r="C118" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>7</v>
       </c>
@@ -2676,13 +2973,16 @@
         <v>126</v>
       </c>
       <c r="C119" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E119" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>7</v>
       </c>
@@ -2690,13 +2990,16 @@
         <v>127</v>
       </c>
       <c r="C120" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E120" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>7</v>
       </c>
@@ -2704,13 +3007,16 @@
         <v>128</v>
       </c>
       <c r="C121" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E121" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>7</v>
       </c>
@@ -2718,13 +3024,16 @@
         <v>129</v>
       </c>
       <c r="C122" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E122" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>7</v>
       </c>
@@ -2732,13 +3041,16 @@
         <v>130</v>
       </c>
       <c r="C123" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E123" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>7</v>
       </c>
@@ -2749,52 +3061,61 @@
         <v>7</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E124" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C125" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C126" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E126" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C127" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E127" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>8</v>
       </c>
@@ -2802,13 +3123,16 @@
         <v>135</v>
       </c>
       <c r="C128" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E128" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>8</v>
       </c>
@@ -2816,13 +3140,16 @@
         <v>136</v>
       </c>
       <c r="C129" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E129" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>8</v>
       </c>
@@ -2830,13 +3157,16 @@
         <v>137</v>
       </c>
       <c r="C130" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E130" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>8</v>
       </c>
@@ -2844,13 +3174,16 @@
         <v>138</v>
       </c>
       <c r="C131" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E131" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>8</v>
       </c>
@@ -2858,13 +3191,13 @@
         <v>139</v>
       </c>
       <c r="C132" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>8</v>
       </c>
@@ -2872,55 +3205,67 @@
         <v>140</v>
       </c>
       <c r="C133" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="E133" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C134" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E134" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C135" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E135" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C136" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E136" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>9</v>
       </c>
@@ -2928,13 +3273,16 @@
         <v>144</v>
       </c>
       <c r="C137" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E137" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>9</v>
       </c>
@@ -2942,13 +3290,16 @@
         <v>145</v>
       </c>
       <c r="C138" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E138" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>9</v>
       </c>
@@ -2959,10 +3310,13 @@
         <v>9</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E139" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>9</v>
       </c>
@@ -2970,13 +3324,16 @@
         <v>147</v>
       </c>
       <c r="C140" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E140" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>9</v>
       </c>
@@ -2984,13 +3341,16 @@
         <v>148</v>
       </c>
       <c r="C141" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E141" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>9</v>
       </c>
@@ -2998,13 +3358,16 @@
         <v>149</v>
       </c>
       <c r="C142" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E142" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>9</v>
       </c>
@@ -3012,55 +3375,67 @@
         <v>150</v>
       </c>
       <c r="C143" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E143" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C144" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E144" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C145" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E145" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C146" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E146" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>10</v>
       </c>
@@ -3068,13 +3443,16 @@
         <v>154</v>
       </c>
       <c r="C147" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E147" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>10</v>
       </c>
@@ -3082,13 +3460,16 @@
         <v>155</v>
       </c>
       <c r="C148" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="E148" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>10</v>
       </c>
@@ -3099,10 +3480,13 @@
         <v>10</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="E149" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>10</v>
       </c>
@@ -3110,29 +3494,32 @@
         <v>157</v>
       </c>
       <c r="C150" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E150" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C151" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>159</v>
@@ -3141,12 +3528,15 @@
         <v>10</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E152" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>160</v>
@@ -3157,8 +3547,11 @@
       <c r="D153" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E153" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>11</v>
       </c>
@@ -3166,13 +3559,16 @@
         <v>161</v>
       </c>
       <c r="C154" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="E154" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>11</v>
       </c>
@@ -3180,13 +3576,16 @@
         <v>162</v>
       </c>
       <c r="C155" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E155" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>11</v>
       </c>
@@ -3194,13 +3593,16 @@
         <v>163</v>
       </c>
       <c r="C156" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E156" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
@@ -3208,13 +3610,16 @@
         <v>164</v>
       </c>
       <c r="C157" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E157" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>11</v>
       </c>
@@ -3225,10 +3630,13 @@
         <v>8</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E158" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>11</v>
       </c>
@@ -3239,10 +3647,13 @@
         <v>8</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="E159" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>11</v>
       </c>
@@ -3250,13 +3661,16 @@
         <v>167</v>
       </c>
       <c r="C160" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E160" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>11</v>
       </c>
@@ -3264,13 +3678,16 @@
         <v>168</v>
       </c>
       <c r="C161" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E161" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>11</v>
       </c>
@@ -3278,13 +3695,16 @@
         <v>169</v>
       </c>
       <c r="C162" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E162" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>11</v>
       </c>
@@ -3292,13 +3712,16 @@
         <v>170</v>
       </c>
       <c r="C163" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E163" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>11</v>
       </c>
@@ -3306,13 +3729,16 @@
         <v>171</v>
       </c>
       <c r="C164" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E164" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>11</v>
       </c>
@@ -3320,13 +3746,16 @@
         <v>172</v>
       </c>
       <c r="C165" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="E165" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>11</v>
       </c>
@@ -3337,10 +3766,13 @@
         <v>5</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="E166" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>11</v>
       </c>
@@ -3348,13 +3780,13 @@
         <v>174</v>
       </c>
       <c r="C167" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>11</v>
       </c>
@@ -3362,13 +3794,16 @@
         <v>175</v>
       </c>
       <c r="C168" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E168" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>11</v>
       </c>
@@ -3376,13 +3811,16 @@
         <v>176</v>
       </c>
       <c r="C169" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="E169" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>11</v>
       </c>
@@ -3390,13 +3828,16 @@
         <v>177</v>
       </c>
       <c r="C170" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E170" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>11</v>
       </c>
@@ -3404,13 +3845,16 @@
         <v>178</v>
       </c>
       <c r="C171" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="E171" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>11</v>
       </c>
@@ -3418,66 +3862,13 @@
         <v>179</v>
       </c>
       <c r="C172" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C173" s="3">
-        <v>2</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C174" s="3">
-        <v>1</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C175" s="3">
-        <v>1</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C176" s="3">
-        <v>10</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
+      </c>
+      <c r="E172" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>